<commit_message>
MVP for buy n get m at x%
</commit_message>
<xml_diff>
--- a/GroceryExcel/GroceryInventory.xlsx
+++ b/GroceryExcel/GroceryInventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="1100" windowWidth="15880" windowHeight="11880" tabRatio="500"/>
+    <workbookView xWindow="11620" yWindow="1900" windowWidth="15880" windowHeight="11880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
   <si>
     <t>Chicken</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Specialty Variable 3</t>
+  </si>
+  <si>
+    <t>nmatx</t>
   </si>
 </sst>
 </file>
@@ -539,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,6 +770,9 @@
       <c r="G11" t="s">
         <v>58</v>
       </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
       <c r="I11">
         <v>3</v>
       </c>
@@ -874,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -885,13 +891,28 @@
         <v>48</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="F17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -911,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>27</v>
       </c>
@@ -928,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>28</v>
       </c>
@@ -945,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -962,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>30</v>
       </c>
@@ -979,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -996,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>31</v>
       </c>
@@ -1013,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>34</v>
       </c>
@@ -1030,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>33</v>
       </c>
@@ -1047,7 +1068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>32</v>
       </c>
@@ -1064,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1084,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>5</v>
       </c>
@@ -1101,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -1118,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -1135,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
MVP for handeling bogo with items with pound units
</commit_message>
<xml_diff>
--- a/GroceryExcel/GroceryInventory.xlsx
+++ b/GroceryExcel/GroceryInventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11620" yWindow="1900" windowWidth="15880" windowHeight="11880" tabRatio="500"/>
+    <workbookView xWindow="9720" yWindow="1900" windowWidth="15880" windowHeight="11880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>Chicken</t>
   </si>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -929,7 +929,16 @@
         <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
MVP for adding more pounds to specialty nforx
</commit_message>
<xml_diff>
--- a/GroceryExcel/GroceryInventory.xlsx
+++ b/GroceryExcel/GroceryInventory.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t>Chicken</t>
   </si>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,7 +1040,19 @@
         <v>0</v>
       </c>
       <c r="F24" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24">
+        <v>6</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Im having major issues with adding lb objects onto other objects and appropriately adjusting price with specialties, I went back to add limits to the sku item specialties
</commit_message>
<xml_diff>
--- a/GroceryExcel/GroceryInventory.xlsx
+++ b/GroceryExcel/GroceryInventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="1900" windowWidth="15880" windowHeight="11880" tabRatio="500"/>
+    <workbookView xWindow="8840" yWindow="2400" windowWidth="15880" windowHeight="11880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>Chicken</t>
   </si>
@@ -542,8 +542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,7 +772,7 @@
         <v>58</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I11">
         <v>3</v>
@@ -955,7 +956,22 @@
         <v>2</v>
       </c>
       <c r="F19" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1046,7 +1062,7 @@
         <v>58</v>
       </c>
       <c r="H24">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I24">
         <v>3</v>

</xml_diff>

<commit_message>
MVP for handeling limits and adding lbs in bogo
</commit_message>
<xml_diff>
--- a/GroceryExcel/GroceryInventory.xlsx
+++ b/GroceryExcel/GroceryInventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="2400" windowWidth="15880" windowHeight="11880" tabRatio="500"/>
+    <workbookView xWindow="400" yWindow="2260" windowWidth="25020" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,138 +41,18 @@
     <t>Seafood</t>
   </si>
   <si>
-    <t>Broccoli</t>
-  </si>
-  <si>
-    <t>Cauliflower</t>
-  </si>
-  <si>
-    <t>Kale</t>
-  </si>
-  <si>
-    <t>Lettuce</t>
-  </si>
-  <si>
-    <t>Breast</t>
-  </si>
-  <si>
-    <t>Legs</t>
-  </si>
-  <si>
-    <t>Thighs</t>
-  </si>
-  <si>
-    <t>Quarters</t>
-  </si>
-  <si>
-    <t>Whole</t>
-  </si>
-  <si>
-    <t>Ground</t>
-  </si>
-  <si>
-    <t>Steak</t>
-  </si>
-  <si>
-    <t>Chops</t>
-  </si>
-  <si>
-    <t>Shoulder</t>
-  </si>
-  <si>
-    <t>Shrimp</t>
-  </si>
-  <si>
-    <t>Scallops</t>
-  </si>
-  <si>
-    <t>Bacon</t>
-  </si>
-  <si>
     <t>lb</t>
   </si>
   <si>
     <t>Dairy/Refridgerated</t>
   </si>
   <si>
-    <t>Eggs</t>
-  </si>
-  <si>
-    <t>Butter</t>
-  </si>
-  <si>
-    <t>Cheese</t>
-  </si>
-  <si>
-    <t>Milk</t>
-  </si>
-  <si>
     <t>Fruits</t>
   </si>
   <si>
-    <t>Banana</t>
-  </si>
-  <si>
-    <t>Strawberries</t>
-  </si>
-  <si>
-    <t>Blueberries</t>
-  </si>
-  <si>
-    <t>Raspberries</t>
-  </si>
-  <si>
-    <t>Grapes</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Lime</t>
-  </si>
-  <si>
-    <t>Lemon</t>
-  </si>
-  <si>
-    <t>Clementine</t>
-  </si>
-  <si>
     <t>Vegetables</t>
   </si>
   <si>
-    <t>Peppers</t>
-  </si>
-  <si>
-    <t>Sweet Potatoe</t>
-  </si>
-  <si>
-    <t>Tomato</t>
-  </si>
-  <si>
-    <t>Asparagus</t>
-  </si>
-  <si>
-    <t>Avocado</t>
-  </si>
-  <si>
-    <t>Carrots</t>
-  </si>
-  <si>
-    <t>Ketchup</t>
-  </si>
-  <si>
-    <t>Mustard</t>
-  </si>
-  <si>
-    <t>Popcorn</t>
-  </si>
-  <si>
-    <t>Pop Tarts</t>
-  </si>
-  <si>
-    <t>Apple</t>
-  </si>
-  <si>
     <t>sku</t>
   </si>
   <si>
@@ -216,6 +96,126 @@
   </si>
   <si>
     <t>nmatx</t>
+  </si>
+  <si>
+    <t>chicken breast</t>
+  </si>
+  <si>
+    <t>chicken legs</t>
+  </si>
+  <si>
+    <t>chicken thighs</t>
+  </si>
+  <si>
+    <t>chicken quarters</t>
+  </si>
+  <si>
+    <t>whole chicken</t>
+  </si>
+  <si>
+    <t>beef ground</t>
+  </si>
+  <si>
+    <t>beef steak</t>
+  </si>
+  <si>
+    <t>beef chops</t>
+  </si>
+  <si>
+    <t>beef shoulder</t>
+  </si>
+  <si>
+    <t>bacon</t>
+  </si>
+  <si>
+    <t>shrimp</t>
+  </si>
+  <si>
+    <t>scallops</t>
+  </si>
+  <si>
+    <t>eggs</t>
+  </si>
+  <si>
+    <t>butter</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>strawberry</t>
+  </si>
+  <si>
+    <t>blueberry</t>
+  </si>
+  <si>
+    <t>raspberry</t>
+  </si>
+  <si>
+    <t>clementine</t>
+  </si>
+  <si>
+    <t>grape</t>
+  </si>
+  <si>
+    <t>lemon</t>
+  </si>
+  <si>
+    <t>lime</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>broccoli</t>
+  </si>
+  <si>
+    <t>cauliflower</t>
+  </si>
+  <si>
+    <t>kale</t>
+  </si>
+  <si>
+    <t>lettuce</t>
+  </si>
+  <si>
+    <t>pepper</t>
+  </si>
+  <si>
+    <t>sweet potato</t>
+  </si>
+  <si>
+    <t>tomato</t>
+  </si>
+  <si>
+    <t>asparagus</t>
+  </si>
+  <si>
+    <t>avocado</t>
+  </si>
+  <si>
+    <t>carrot</t>
+  </si>
+  <si>
+    <t>ketchup</t>
+  </si>
+  <si>
+    <t>mustard</t>
+  </si>
+  <si>
+    <t>popcorn</t>
+  </si>
+  <si>
+    <t>pop tart</t>
   </si>
 </sst>
 </file>
@@ -267,7 +267,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -275,6 +293,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K41" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:K41"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Category"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="3" name="Price"/>
+    <tableColumn id="4" name="Units"/>
+    <tableColumn id="5" name="Markdown"/>
+    <tableColumn id="6" name="Has Specialty"/>
+    <tableColumn id="7" name="Type of Specialty"/>
+    <tableColumn id="8" name="Limit"/>
+    <tableColumn id="9" name="Specialty Variable 1"/>
+    <tableColumn id="10" name="Specialty Variable 2"/>
+    <tableColumn id="11" name="Specialty Variable 3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,52 +580,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="11" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -595,13 +637,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1">
-        <v>2.99</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -612,13 +654,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C3">
-        <v>1.99</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -629,13 +671,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C4">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -646,13 +688,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>1.49</v>
+        <v>1.5</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -663,13 +705,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C6">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -683,13 +725,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>2.99</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -700,13 +742,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C8">
-        <v>5.49</v>
+        <v>5.5</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -720,13 +762,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>1.99</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -737,13 +779,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C10">
-        <v>2.4900000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -754,13 +796,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -769,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="H11">
         <v>9</v>
@@ -786,13 +828,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C12">
-        <v>5.99</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -803,13 +845,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C13">
-        <v>9.99</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -820,16 +862,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C14">
-        <v>1.79</v>
+        <v>1.8</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -840,22 +882,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C15">
-        <v>3.19</v>
+        <v>3.2</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E15">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -866,13 +908,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C16">
-        <v>3.99</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -883,25 +925,25 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C17">
-        <v>3.49</v>
+        <v>3.5</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E17">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="H17">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -915,16 +957,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -933,7 +975,7 @@
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="H18">
         <v>6</v>
@@ -944,13 +986,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -959,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="H19">
         <v>6</v>
@@ -976,13 +1018,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -993,13 +1035,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C21">
-        <v>1.99</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1010,13 +1052,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C22">
-        <v>1.99</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1027,13 +1069,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C23">
-        <v>3.99</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1044,13 +1086,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1059,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="H24">
         <v>9</v>
@@ -1073,13 +1115,13 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C25">
-        <v>0.69</v>
+        <v>0.7</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1090,13 +1132,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C26">
         <v>0.5</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1107,13 +1149,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C27">
-        <v>1.99</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1124,16 +1166,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C28">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1144,13 +1186,13 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C29">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1161,13 +1203,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C30">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1178,13 +1220,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="C31">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1195,13 +1237,13 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C32">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1212,13 +1254,13 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C33">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1229,13 +1271,13 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C34">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1246,13 +1288,13 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C35">
-        <v>2.99</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1263,13 +1305,13 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C36">
         <v>1.25</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1280,13 +1322,13 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C37">
         <v>0.65</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1297,13 +1339,13 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C38">
-        <v>2.4900000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1314,13 +1356,13 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C39">
-        <v>1.79</v>
+        <v>1.8</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1331,13 +1373,13 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C40">
-        <v>3.49</v>
+        <v>3.5</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1348,13 +1390,13 @@
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C41">
-        <v>3.49</v>
+        <v>3.5</v>
       </c>
       <c r="D41" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1365,5 +1407,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated formatting for dollar amounts being printed
</commit_message>
<xml_diff>
--- a/GroceryExcel/GroceryInventory.xlsx
+++ b/GroceryExcel/GroceryInventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="400" yWindow="2260" windowWidth="25020" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="620" windowWidth="25020" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -267,7 +267,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -296,14 +302,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K41" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K41" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:K41"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Category"/>
     <tableColumn id="2" name="Name"/>
-    <tableColumn id="3" name="Price"/>
+    <tableColumn id="3" name="Price" dataDxfId="1"/>
     <tableColumn id="4" name="Units"/>
-    <tableColumn id="5" name="Markdown"/>
+    <tableColumn id="5" name="Markdown" dataDxfId="0"/>
     <tableColumn id="6" name="Has Specialty"/>
     <tableColumn id="7" name="Type of Specialty"/>
     <tableColumn id="8" name="Limit"/>
@@ -581,8 +587,8 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,7 +651,7 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" t="b">
@@ -656,13 +662,13 @@
       <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" t="b">
@@ -673,13 +679,13 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1.5</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" t="b">
@@ -690,13 +696,13 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1.5</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" t="b">
@@ -707,13 +713,13 @@
       <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1.2</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" t="b">
@@ -727,13 +733,13 @@
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>3</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>0</v>
       </c>
       <c r="F7" t="b">
@@ -744,13 +750,13 @@
       <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>5.5</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>0</v>
       </c>
       <c r="F8" t="b">
@@ -764,13 +770,13 @@
       <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>2</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>0</v>
       </c>
       <c r="F9" t="b">
@@ -781,13 +787,13 @@
       <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>2.5</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>0</v>
       </c>
       <c r="F10" t="b">
@@ -798,13 +804,13 @@
       <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>4</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>0</v>
       </c>
       <c r="F11" t="b">
@@ -830,13 +836,13 @@
       <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>6</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" t="b">
@@ -847,13 +853,13 @@
       <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>10</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>0</v>
       </c>
       <c r="F13" t="b">
@@ -867,13 +873,13 @@
       <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>1.8</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14" t="b">
@@ -884,13 +890,13 @@
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>3.2</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>0.2</v>
       </c>
       <c r="F15" t="b">
@@ -910,13 +916,13 @@
       <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>4</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>0</v>
       </c>
       <c r="F16" t="b">
@@ -927,13 +933,13 @@
       <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>3.5</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>0.5</v>
       </c>
       <c r="F17" t="b">
@@ -962,13 +968,13 @@
       <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>5</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" t="b">
@@ -988,13 +994,13 @@
       <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>4</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>2</v>
       </c>
       <c r="F19" t="b">
@@ -1020,13 +1026,13 @@
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>0</v>
       </c>
       <c r="F20" t="b">
@@ -1037,13 +1043,13 @@
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>0</v>
       </c>
       <c r="F21" t="b">
@@ -1054,13 +1060,13 @@
       <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" t="b">
@@ -1071,13 +1077,13 @@
       <c r="B23" t="s">
         <v>44</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>4</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>0</v>
       </c>
       <c r="F23" t="b">
@@ -1088,13 +1094,13 @@
       <c r="B24" t="s">
         <v>45</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>3</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24" t="b">
@@ -1117,13 +1123,13 @@
       <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>0.7</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>0</v>
       </c>
       <c r="F25" t="b">
@@ -1134,13 +1140,13 @@
       <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>0.5</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" t="b">
@@ -1151,13 +1157,13 @@
       <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27" t="b">
@@ -1171,13 +1177,13 @@
       <c r="B28" t="s">
         <v>49</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <v>1</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="F28" t="b">
@@ -1188,13 +1194,13 @@
       <c r="B29" t="s">
         <v>50</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" t="b">
@@ -1205,13 +1211,13 @@
       <c r="B30" t="s">
         <v>51</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" t="b">
@@ -1222,13 +1228,13 @@
       <c r="B31" t="s">
         <v>52</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>0</v>
       </c>
       <c r="F31" t="b">
@@ -1239,13 +1245,13 @@
       <c r="B32" t="s">
         <v>53</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" t="b">
@@ -1256,13 +1262,13 @@
       <c r="B33" t="s">
         <v>54</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" t="b">
@@ -1273,13 +1279,13 @@
       <c r="B34" t="s">
         <v>55</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>0</v>
       </c>
       <c r="F34" t="b">
@@ -1290,13 +1296,13 @@
       <c r="B35" t="s">
         <v>56</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
         <v>3</v>
       </c>
       <c r="D35" t="s">
         <v>4</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" t="b">
@@ -1307,13 +1313,13 @@
       <c r="B36" t="s">
         <v>57</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
         <v>1.25</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>0</v>
       </c>
       <c r="F36" t="b">
@@ -1324,13 +1330,13 @@
       <c r="B37" t="s">
         <v>58</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>0.65</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>0</v>
       </c>
       <c r="F37" t="b">
@@ -1341,13 +1347,13 @@
       <c r="B38" t="s">
         <v>59</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>2.5</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>0</v>
       </c>
       <c r="F38" t="b">
@@ -1358,13 +1364,13 @@
       <c r="B39" t="s">
         <v>60</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>1.8</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>0</v>
       </c>
       <c r="F39" t="b">
@@ -1375,13 +1381,13 @@
       <c r="B40" t="s">
         <v>61</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>3.5</v>
       </c>
       <c r="D40" t="s">
         <v>8</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>0</v>
       </c>
       <c r="F40" t="b">
@@ -1392,13 +1398,13 @@
       <c r="B41" t="s">
         <v>62</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>3.5</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>0</v>
       </c>
       <c r="F41" t="b">

</xml_diff>

<commit_message>
some formatting adjustments involved with the printing specialties to strings
</commit_message>
<xml_diff>
--- a/GroceryExcel/GroceryInventory.xlsx
+++ b/GroceryExcel/GroceryInventory.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>Chicken</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>pop tart</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -587,8 +590,8 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,6 +660,9 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -674,6 +680,9 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -691,6 +700,9 @@
       <c r="F4" t="b">
         <v>0</v>
       </c>
+      <c r="G4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -708,6 +720,9 @@
       <c r="F5" t="b">
         <v>0</v>
       </c>
+      <c r="G5" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
@@ -725,6 +740,9 @@
       <c r="F6" t="b">
         <v>0</v>
       </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -744,6 +762,9 @@
       </c>
       <c r="F7" t="b">
         <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -762,6 +783,9 @@
       <c r="F8" t="b">
         <v>0</v>
       </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -782,6 +806,9 @@
       <c r="F9" t="b">
         <v>0</v>
       </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
@@ -799,6 +826,9 @@
       <c r="F10" t="b">
         <v>0</v>
       </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -848,6 +878,9 @@
       <c r="F12" t="b">
         <v>0</v>
       </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
@@ -865,6 +898,9 @@
       <c r="F13" t="b">
         <v>0</v>
       </c>
+      <c r="G13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -885,6 +921,9 @@
       <c r="F14" t="b">
         <v>0</v>
       </c>
+      <c r="G14" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -928,6 +967,9 @@
       <c r="F16" t="b">
         <v>0</v>
       </c>
+      <c r="G16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
@@ -1038,6 +1080,9 @@
       <c r="F20" t="b">
         <v>1</v>
       </c>
+      <c r="G20" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
@@ -1055,6 +1100,9 @@
       <c r="F21" t="b">
         <v>0</v>
       </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
@@ -1072,6 +1120,9 @@
       <c r="F22" t="b">
         <v>0</v>
       </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
@@ -1089,6 +1140,9 @@
       <c r="F23" t="b">
         <v>0</v>
       </c>
+      <c r="G23" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
@@ -1135,6 +1189,9 @@
       <c r="F25" t="b">
         <v>0</v>
       </c>
+      <c r="G25" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
@@ -1152,6 +1209,9 @@
       <c r="F26" t="b">
         <v>0</v>
       </c>
+      <c r="G26" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
@@ -1169,6 +1229,9 @@
       <c r="F27" t="b">
         <v>0</v>
       </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1189,6 +1252,9 @@
       <c r="F28" t="b">
         <v>0</v>
       </c>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
@@ -1206,6 +1272,9 @@
       <c r="F29" t="b">
         <v>0</v>
       </c>
+      <c r="G29" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
@@ -1223,6 +1292,9 @@
       <c r="F30" t="b">
         <v>0</v>
       </c>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
@@ -1240,6 +1312,9 @@
       <c r="F31" t="b">
         <v>0</v>
       </c>
+      <c r="G31" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
@@ -1257,8 +1332,11 @@
       <c r="F32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>54</v>
       </c>
@@ -1274,8 +1352,11 @@
       <c r="F33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>55</v>
       </c>
@@ -1291,8 +1372,11 @@
       <c r="F34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>56</v>
       </c>
@@ -1308,8 +1392,11 @@
       <c r="F35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>57</v>
       </c>
@@ -1325,8 +1412,11 @@
       <c r="F36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>58</v>
       </c>
@@ -1342,8 +1432,11 @@
       <c r="F37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>59</v>
       </c>
@@ -1359,8 +1452,11 @@
       <c r="F38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>60</v>
       </c>
@@ -1376,8 +1472,11 @@
       <c r="F39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>61</v>
       </c>
@@ -1393,8 +1492,11 @@
       <c r="F40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>62</v>
       </c>
@@ -1409,6 +1511,9 @@
       </c>
       <c r="F41" t="b">
         <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mvp for adding lb objects for nmatx
</commit_message>
<xml_diff>
--- a/GroceryExcel/GroceryInventory.xlsx
+++ b/GroceryExcel/GroceryInventory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="620" windowWidth="25020" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="2380" yWindow="2460" windowWidth="25020" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -590,8 +590,8 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25:G41"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -1052,7 +1052,7 @@
         <v>22</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I19">
         <v>3</v>

</xml_diff>